<commit_message>
added cmi_2024 to circuit dataframe
</commit_message>
<xml_diff>
--- a/Data/circuit_outages_ibec.xlsx
+++ b/Data/circuit_outages_ibec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Cal Poly MISSA ITC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardogutierrez/Desktop/ITC_2025/itty-bitty-electric-company-proposal/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBD66FD9-40A1-4228-BD8A-AFFE35B150B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3644B668-EB0F-0740-A7A6-2CAD1D364EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{67E1BD3D-E95E-4409-B542-F5A0F1E2953B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20740" windowHeight="11160" xr2:uid="{67E1BD3D-E95E-4409-B542-F5A0F1E2953B}"/>
   </bookViews>
   <sheets>
     <sheet name="Circuit Outage" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -278,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -617,24 +617,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0032BE82-69C4-4403-BCCC-DC8484F7BB89}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:I101"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -657,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -682,7 +682,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -784,7 +784,7 @@
         <v>3198</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>2</v>
       </c>
@@ -809,7 +809,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -911,7 +911,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -936,7 +936,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>3</v>
       </c>
@@ -961,7 +961,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>4</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>5</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>45320</v>
       </c>
       <c r="D20" s="3">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E20" t="str">
         <f>VLOOKUP(D20,LookUp!L$2:M$9,2)</f>
@@ -1140,7 +1140,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>5</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>5</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>5</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>5</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>6</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>6</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>6</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>7</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>7</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>7</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>7</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>7</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>7</v>
       </c>
@@ -1496,7 +1496,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>8</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>8</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>9</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>9</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>9</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>9</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>9</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>9</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>9</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>9</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>9</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>10</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>10</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="14"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>11</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>11</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>11</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>11</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>11</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>11</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>11</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>11</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>11</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>12</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>12</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>12</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="H61" s="13"/>
       <c r="I61" s="14"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>13</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>13</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>13</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>13</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>13</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>13</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>13</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>13</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>13</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="14"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>14</v>
       </c>
@@ -2443,7 +2443,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="14"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>15</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>15</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="14"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>16</v>
       </c>
@@ -2522,7 +2522,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="14"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>17</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>17</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>17</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>17</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>17</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>17</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>17</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="14"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>18</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>18</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="H83" s="13"/>
       <c r="I83" s="14"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>19</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>19</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>19</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>19</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>19</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>19</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>19</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>19</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>19</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>19</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="H93" s="13"/>
       <c r="I93" s="14"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>20</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="H94" s="13"/>
       <c r="I94" s="14"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>21</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>21</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>21</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>21</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>21</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>21</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>21</v>
       </c>
@@ -3220,26 +3220,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BB01FE-E4DE-49B7-B420-E065E461E21B}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="O3" s="11"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="O5" s="11"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>

</xml_diff>